<commit_message>
Remove projector enhancement (does not improve results)
</commit_message>
<xml_diff>
--- a/data/inference_images/inference_results.xlsx
+++ b/data/inference_images/inference_results.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Vie Professionnelle\GitHub Projects\CV-image-captioning-clip-gpt2-aws\data\inference_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D75E051-6550-470C-B29B-CE3BB981CFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F8B4B9-58B9-47DB-9837-FE07C43FC644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{49327151-6212-4F5F-B97F-F963B41DC1CE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{49327151-6212-4F5F-B97F-F963B41DC1CE}"/>
   </bookViews>
   <sheets>
     <sheet name="inference_results" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -884,7 +884,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -893,15 +893,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -947,14 +941,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -973,13 +960,6 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1799,7 +1779,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C132D6A8-625E-48E8-91A7-FC05B168214E}" name="Tableau croisé dynamique3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C132D6A8-625E-48E8-91A7-FC05B168214E}" name="Tableau croisé dynamique3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H7:I14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -1850,7 +1830,7 @@
     <dataField name="Somme de score" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="5">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="4">
@@ -1862,7 +1842,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="4">
@@ -2227,8 +2207,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2360,7 +2340,7 @@
       <c r="H8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8">
         <v>1</v>
       </c>
     </row>
@@ -2380,7 +2360,7 @@
       <c r="H9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9">
         <v>20</v>
       </c>
     </row>
@@ -2397,10 +2377,10 @@
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10">
         <v>24</v>
       </c>
     </row>
@@ -2417,10 +2397,10 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="2">
         <v>26</v>
       </c>
     </row>
@@ -2437,10 +2417,10 @@
       <c r="D12">
         <v>2</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="2">
         <v>26</v>
       </c>
     </row>
@@ -2457,10 +2437,10 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13">
         <v>24</v>
       </c>
     </row>
@@ -2480,7 +2460,7 @@
       <c r="H14" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
push new inference images
</commit_message>
<xml_diff>
--- a/data/inference_images/inference_results.xlsx
+++ b/data/inference_images/inference_results.xlsx
@@ -2,28 +2,31 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Vie Professionnelle\GitHub Projects\CV-image-captioning-clip-gpt2-aws\data\inference_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F8B4B9-58B9-47DB-9837-FE07C43FC644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E88C1DD-D8AB-4F14-8687-A4533BD05D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{49327151-6212-4F5F-B97F-F963B41DC1CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B9F52076-50CF-4234-A6EE-BD5871CA9C28}"/>
   </bookViews>
   <sheets>
     <sheet name="inference_results" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">inference_results!$A$1:$D$163</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="5" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="156">
   <si>
     <t>image_id</t>
   </si>
@@ -166,6 +169,45 @@
     <t>A cat laying on a bed with a remote control.</t>
   </si>
   <si>
+    <t>cake.jpg</t>
+  </si>
+  <si>
+    <t>A man is riding a skateboard on a city street.</t>
+  </si>
+  <si>
+    <t>A birthday cake with a birthday candle on top of it.</t>
+  </si>
+  <si>
+    <t>A birthday cake with candles on top of it.</t>
+  </si>
+  <si>
+    <t>A blue and white cake on a table.</t>
+  </si>
+  <si>
+    <t>A group of people standing around a cake.</t>
+  </si>
+  <si>
+    <t>A cake that is sitting on top of a table.</t>
+  </si>
+  <si>
+    <t>chess.jpg</t>
+  </si>
+  <si>
+    <t>A woman sitting at a table with a plate of food.</t>
+  </si>
+  <si>
+    <t>A group of women sitting at a table with food.</t>
+  </si>
+  <si>
+    <t>A couple of women sitting on top of a table.</t>
+  </si>
+  <si>
+    <t>A group of women sitting at a table with a group of children.</t>
+  </si>
+  <si>
+    <t>A group of people sitting around a table with plates of food.</t>
+  </si>
+  <si>
     <t>cs2.jpg</t>
   </si>
   <si>
@@ -193,6 +235,24 @@
     <t xml:space="preserve">a close up of some food on a table </t>
   </si>
   <si>
+    <t>lemans_race.jpg</t>
+  </si>
+  <si>
+    <t>A group of people standing on top of a cruise ship.</t>
+  </si>
+  <si>
+    <t>A man standing in front of a gas station.</t>
+  </si>
+  <si>
+    <t>A man standing next to a parked motorcycle.</t>
+  </si>
+  <si>
+    <t>A man standing next to a blue and white truck.</t>
+  </si>
+  <si>
+    <t>A man standing next to a man on a motorcycle.</t>
+  </si>
+  <si>
     <t>match.jpg</t>
   </si>
   <si>
@@ -232,6 +292,24 @@
     <t>A large building with a clock on the top of it.</t>
   </si>
   <si>
+    <t>pastries.jpg</t>
+  </si>
+  <si>
+    <t>A man standing in front of a cart filled with bananas.</t>
+  </si>
+  <si>
+    <t>A display case filled with lots of different kinds of donuts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A display case filled with lots of donuts. </t>
+  </si>
+  <si>
+    <t>A woman standing in front of a display of donuts.</t>
+  </si>
+  <si>
+    <t>A group of people standing around a display of donuts.</t>
+  </si>
+  <si>
     <t>psg_stadium.jpg</t>
   </si>
   <si>
@@ -310,9 +388,6 @@
     <t>A Christmas tree in front of a Christmas tree.</t>
   </si>
   <si>
-    <t>A teddy bear sitting on top of a Christmas tree.</t>
-  </si>
-  <si>
     <t>A Christmas tree sitting on top of a Christmas tree.</t>
   </si>
   <si>
@@ -334,6 +409,24 @@
     <t>A group of men playing frisbee in a park.</t>
   </si>
   <si>
+    <t>surgery.jpg</t>
+  </si>
+  <si>
+    <t>A group of people sitting around a table with laptops.</t>
+  </si>
+  <si>
+    <t>A group of people in a hospital gown.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A group of surgeons performing surgery on a patient. </t>
+  </si>
+  <si>
+    <t>A group of surgeons in a hospital room.</t>
+  </si>
+  <si>
+    <t>A group of surgeons in a hospital setting.</t>
+  </si>
+  <si>
     <t>tennis.jpg</t>
   </si>
   <si>
@@ -364,16 +457,34 @@
     <t>A model of a toy train on a table.</t>
   </si>
   <si>
+    <t>tree_antibes.jpg</t>
+  </si>
+  <si>
+    <t>A giraffe standing next to a tree in front of a tree.</t>
+  </si>
+  <si>
+    <t>A tree that is in the middle of a grassy field.</t>
+  </si>
+  <si>
+    <t>A tree that has a bunch of leaves on it.</t>
+  </si>
+  <si>
+    <t>A large tree in the middle of a grassy field.</t>
+  </si>
+  <si>
+    <t>A tree in the middle of a lush green field.</t>
+  </si>
+  <si>
     <t>family.png</t>
   </si>
   <si>
-    <t>A group of people sitting around a table with laptops.</t>
-  </si>
-  <si>
     <t>A group of people sitting at a table with a laptop computer.</t>
   </si>
   <si>
     <t>score</t>
+  </si>
+  <si>
+    <t>A teddy bear sitting next to a Christmas tree.</t>
   </si>
   <si>
     <t>Étiquettes de lignes</t>
@@ -707,13 +818,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -724,7 +835,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -839,6 +950,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -884,18 +1010,30 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -941,11 +1079,46 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -958,15 +1131,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -984,9 +1150,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Moetez Lahdhiri" refreshedDate="45865.061802893521" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="126" xr:uid="{CFB24320-9B2B-46CF-AF4A-5C807A81FC66}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Moetez Lahdhiri" refreshedDate="45865.47450196759" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="162" xr:uid="{17E0E282-2505-4A89-A17F-ABDC347B4BF0}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:D127" sheet="inference_results"/>
+    <worksheetSource ref="A1:D163" sheet="inference_results"/>
   </cacheSource>
   <cacheFields count="4">
     <cacheField name="image_id" numFmtId="0">
@@ -1018,7 +1184,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="126">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="162">
   <r>
     <s v="airbnb.jpg"/>
     <x v="0"/>
@@ -1053,7 +1219,7 @@
     <s v="airbnb.jpg"/>
     <x v="5"/>
     <s v="A kitchen with a stove, sink, microwave and refrigerator."/>
-    <n v="2"/>
+    <n v="1"/>
   </r>
   <r>
     <s v="amg_c63.jpg"/>
@@ -1155,7 +1321,7 @@
     <s v="antibes_2.jpg"/>
     <x v="4"/>
     <s v="A red and white street sign sitting next to a building."/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <s v="antibes_2.jpg"/>
@@ -1191,13 +1357,13 @@
     <s v="baby_yoda.jpg"/>
     <x v="4"/>
     <s v="A man holding a stuffed animal in his hand."/>
-    <n v="1"/>
+    <n v="2"/>
   </r>
   <r>
     <s v="baby_yoda.jpg"/>
     <x v="5"/>
     <s v="A man is holding a stuffed animal in his hand."/>
-    <n v="1"/>
+    <n v="2"/>
   </r>
   <r>
     <s v="beach.jpg"/>
@@ -1209,7 +1375,7 @@
     <s v="beach.jpg"/>
     <x v="1"/>
     <s v="A group of people sitting on a beach with umbrellas."/>
-    <n v="2"/>
+    <n v="1"/>
   </r>
   <r>
     <s v="beach.jpg"/>
@@ -1245,7 +1411,7 @@
     <s v="bibi.jpg"/>
     <x v="1"/>
     <s v="A black cat sitting on top of a toilet bowl."/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <s v="bibi.jpg"/>
@@ -1269,13 +1435,85 @@
     <s v="bibi.jpg"/>
     <x v="5"/>
     <s v="A cat laying on a bed with a remote control."/>
-    <n v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="cake.jpg"/>
+    <x v="0"/>
+    <s v="A man is riding a skateboard on a city street."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="cake.jpg"/>
+    <x v="1"/>
+    <s v="A birthday cake with a birthday candle on top of it."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="cake.jpg"/>
+    <x v="2"/>
+    <s v="A birthday cake with candles on top of it."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="cake.jpg"/>
+    <x v="3"/>
+    <s v="A blue and white cake on a table."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="cake.jpg"/>
+    <x v="4"/>
+    <s v="A group of people standing around a cake."/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="cake.jpg"/>
+    <x v="5"/>
+    <s v="A cake that is sitting on top of a table."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="chess.jpg"/>
+    <x v="0"/>
+    <s v="A man is riding a skateboard on a city street."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="chess.jpg"/>
+    <x v="1"/>
+    <s v="A woman sitting at a table with a plate of food."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="chess.jpg"/>
+    <x v="2"/>
+    <s v="A group of women sitting at a table with food."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="chess.jpg"/>
+    <x v="3"/>
+    <s v="A couple of women sitting on top of a table."/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="chess.jpg"/>
+    <x v="4"/>
+    <s v="A group of women sitting at a table with a group of children."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="chess.jpg"/>
+    <x v="5"/>
+    <s v="A group of people sitting around a table with plates of food."/>
+    <n v="0"/>
   </r>
   <r>
     <s v="cs2.jpg"/>
     <x v="0"/>
     <s v="A group of people sitting around a table."/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <s v="cs2.jpg"/>
@@ -1342,6 +1580,42 @@
     <x v="5"/>
     <s v="a close up of some food on a table "/>
     <n v="0"/>
+  </r>
+  <r>
+    <s v="lemans_race.jpg"/>
+    <x v="0"/>
+    <s v="A man riding a skateboard on a city street."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="lemans_race.jpg"/>
+    <x v="1"/>
+    <s v="A group of people standing on top of a cruise ship."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="lemans_race.jpg"/>
+    <x v="2"/>
+    <s v="A man standing in front of a gas station."/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="lemans_race.jpg"/>
+    <x v="3"/>
+    <s v="A man standing next to a parked motorcycle."/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="lemans_race.jpg"/>
+    <x v="4"/>
+    <s v="A man standing next to a blue and white truck."/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="lemans_race.jpg"/>
+    <x v="5"/>
+    <s v="A man standing next to a man on a motorcycle."/>
+    <n v="1"/>
   </r>
   <r>
     <s v="match.jpg"/>
@@ -1452,6 +1726,42 @@
     <n v="1"/>
   </r>
   <r>
+    <s v="pastries.jpg"/>
+    <x v="0"/>
+    <s v="A cat is sitting on top of a chair."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="pastries.jpg"/>
+    <x v="1"/>
+    <s v="A man standing in front of a cart filled with bananas."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="pastries.jpg"/>
+    <x v="2"/>
+    <s v="A display case filled with lots of different kinds of donuts."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="pastries.jpg"/>
+    <x v="3"/>
+    <s v="A display case filled with lots of donuts. "/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="pastries.jpg"/>
+    <x v="4"/>
+    <s v="A woman standing in front of a display of donuts."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="pastries.jpg"/>
+    <x v="5"/>
+    <s v="A group of people standing around a display of donuts."/>
+    <n v="2"/>
+  </r>
+  <r>
     <s v="psg_stadium.jpg"/>
     <x v="0"/>
     <s v="A man riding a skateboard on a city street."/>
@@ -1503,25 +1813,25 @@
     <s v="shopping.jpg"/>
     <x v="2"/>
     <s v="A woman and a man walking down a street."/>
-    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <s v="shopping.jpg"/>
     <x v="3"/>
     <s v="A woman and a man walking down a street. "/>
-    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <s v="shopping.jpg"/>
     <x v="4"/>
     <s v="A woman and a man walking down a street."/>
-    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <s v="shopping.jpg"/>
     <x v="5"/>
     <s v="A group of people walking down a street."/>
-    <n v="0"/>
+    <n v="2"/>
   </r>
   <r>
     <s v="sofia.jpg"/>
@@ -1610,13 +1920,13 @@
   <r>
     <s v="sofia_2.jpg"/>
     <x v="2"/>
-    <s v="A teddy bear sitting on top of a Christmas tree."/>
+    <s v="A teddy bear sitting next to a Christmas tree."/>
     <n v="1"/>
   </r>
   <r>
     <s v="sofia_2.jpg"/>
     <x v="3"/>
-    <s v="A teddy bear sitting on top of a Christmas tree."/>
+    <s v="A teddy bear sitting next to a Christmas tree."/>
     <n v="1"/>
   </r>
   <r>
@@ -1628,7 +1938,7 @@
   <r>
     <s v="sofia_2.jpg"/>
     <x v="5"/>
-    <s v="A teddy bear sitting on top of a Christmas tree."/>
+    <s v="A teddy bear sitting next to a Christmas tree."/>
     <n v="1"/>
   </r>
   <r>
@@ -1641,13 +1951,13 @@
     <s v="sport.jpg"/>
     <x v="1"/>
     <s v="A group of people playing frisbee in a park."/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <s v="sport.jpg"/>
     <x v="2"/>
     <s v="A group of young men playing frisbee in a park."/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <s v="sport.jpg"/>
@@ -1659,13 +1969,49 @@
     <s v="sport.jpg"/>
     <x v="4"/>
     <s v="A group of young men playing with a Frisbee in a park."/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <s v="sport.jpg"/>
     <x v="5"/>
     <s v="A group of men playing frisbee in a park."/>
-    <n v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="surgery.jpg"/>
+    <x v="0"/>
+    <s v="A man riding a skateboard on a city street."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="surgery.jpg"/>
+    <x v="1"/>
+    <s v="A group of people sitting around a table with laptops."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="surgery.jpg"/>
+    <x v="2"/>
+    <s v="A group of people in a hospital gown."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="surgery.jpg"/>
+    <x v="3"/>
+    <s v="A group of surgeons performing surgery on a patient. "/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="surgery.jpg"/>
+    <x v="4"/>
+    <s v="A group of surgeons in a hospital room."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="surgery.jpg"/>
+    <x v="5"/>
+    <s v="A group of surgeons in a hospital setting."/>
+    <n v="2"/>
   </r>
   <r>
     <s v="tennis.jpg"/>
@@ -1740,6 +2086,42 @@
     <n v="1"/>
   </r>
   <r>
+    <s v="tree_antibes.jpg"/>
+    <x v="0"/>
+    <s v="A man riding a skateboard on a city street."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="tree_antibes.jpg"/>
+    <x v="1"/>
+    <s v="A giraffe standing next to a tree in front of a tree."/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="tree_antibes.jpg"/>
+    <x v="2"/>
+    <s v="A tree that is in the middle of a grassy field."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="tree_antibes.jpg"/>
+    <x v="3"/>
+    <s v="A tree that has a bunch of leaves on it."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="tree_antibes.jpg"/>
+    <x v="4"/>
+    <s v="A large tree in the middle of a grassy field."/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="tree_antibes.jpg"/>
+    <x v="5"/>
+    <s v="A tree in the middle of a lush green field."/>
+    <n v="2"/>
+  </r>
+  <r>
     <s v="family.png"/>
     <x v="0"/>
     <s v="A man riding a skateboard on a city street."/>
@@ -1779,8 +2161,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C132D6A8-625E-48E8-91A7-FC05B168214E}" name="Tableau croisé dynamique3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="H7:I14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B03A5A9C-43FA-48DC-8DFD-1DFDB74DD6EA}" name="Tableau croisé dynamique2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="G5:H12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -1829,15 +2211,48 @@
   <dataFields count="1">
     <dataField name="Somme de score" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="4">
+  <formats count="8">
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="4">
+          <reference field="1" count="1">
             <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
@@ -1845,11 +2260,8 @@
     <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="4">
+          <reference field="1" count="1">
             <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
@@ -1857,9 +2269,8 @@
     <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="2">
-            <x v="3"/>
-            <x v="4"/>
+          <reference field="1" count="1">
+            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
@@ -1867,9 +2278,8 @@
     <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="2">
-            <x v="3"/>
-            <x v="4"/>
+          <reference field="1" count="1">
+            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
@@ -2203,129 +2613,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C714EE76-FFD3-4491-BDEC-3689CB29DBC8}">
-  <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:I127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBAC580C-6DBF-4BD9-8363-2556C5C8014C}">
+  <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="G5" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="I7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2334,118 +2755,112 @@
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="6">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="2">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="2">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2454,18 +2869,12 @@
       <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I14">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2474,68 +2883,68 @@
       <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2544,82 +2953,82 @@
       <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2628,12 +3037,12 @@
       <c r="C26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2642,12 +3051,12 @@
       <c r="C27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2656,12 +3065,12 @@
       <c r="C28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2670,40 +3079,40 @@
       <c r="C29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D30">
-        <v>1</v>
+      <c r="D30" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D31">
-        <v>1</v>
+      <c r="D31" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2712,82 +3121,82 @@
       <c r="C32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D33">
-        <v>2</v>
+      <c r="D33" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2796,419 +3205,419 @@
       <c r="C38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="2" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="2" t="s">
+      <c r="C46" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="2" t="s">
+      <c r="C47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="2" t="s">
+      <c r="C48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49">
+      <c r="C49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>50</v>
+      <c r="A50" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50">
+        <v>48</v>
+      </c>
+      <c r="D50" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>50</v>
+      <c r="A51" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51">
+        <v>55</v>
+      </c>
+      <c r="D51" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>50</v>
+      <c r="A52" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D52">
+        <v>56</v>
+      </c>
+      <c r="D52" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>50</v>
+      <c r="A53" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>50</v>
+      <c r="A54" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>50</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D55">
+        <v>59</v>
+      </c>
+      <c r="D55" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>56</v>
+      <c r="A56" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56">
+        <v>61</v>
+      </c>
+      <c r="D56" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" s="2" t="s">
+      <c r="A57" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57">
+      <c r="C57" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D57" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="2" t="s">
+      <c r="A58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D58">
+      <c r="C58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>56</v>
-      </c>
-      <c r="B59" s="2" t="s">
+      <c r="A59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D59">
+      <c r="C59" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D59" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="2" t="s">
+      <c r="A60" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D60">
+      <c r="C60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>56</v>
-      </c>
-      <c r="B61" s="2" t="s">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D61">
+      <c r="C61" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>60</v>
+      <c r="A62" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="D62" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>60</v>
+      <c r="A63" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D63">
+        <v>64</v>
+      </c>
+      <c r="D63" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>60</v>
+      <c r="A64" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D64">
+        <v>65</v>
+      </c>
+      <c r="D64" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>60</v>
+      <c r="A65" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>60</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D66">
+        <v>67</v>
+      </c>
+      <c r="D66" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>60</v>
+      <c r="A67" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D67">
+        <v>68</v>
+      </c>
+      <c r="D67" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>64</v>
+      <c r="A68" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>4</v>
@@ -3216,83 +3625,83 @@
       <c r="C68" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" s="2" t="s">
+      <c r="A69" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D69">
-        <v>2</v>
+      <c r="C69" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>64</v>
-      </c>
-      <c r="B70" s="3" t="s">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D70">
+      <c r="C70" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D70" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B71" s="2" t="s">
+      <c r="A71" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D71">
-        <v>2</v>
+      <c r="C71" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>64</v>
-      </c>
-      <c r="B72" s="2" t="s">
+      <c r="A72" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D72">
-        <v>2</v>
+      <c r="C72" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>64</v>
-      </c>
-      <c r="B73" s="3" t="s">
+      <c r="A73" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D73">
+      <c r="C73" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D73" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>69</v>
+      <c r="A74" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>4</v>
@@ -3300,83 +3709,83 @@
       <c r="C74" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>69</v>
-      </c>
-      <c r="B75" s="3" t="s">
+      <c r="A75" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D75">
-        <v>1</v>
+      <c r="C75" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D75" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>69</v>
-      </c>
-      <c r="B76" s="3" t="s">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
+      <c r="C76" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D76" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>69</v>
-      </c>
-      <c r="B77" s="2" t="s">
+      <c r="A77" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D77">
+      <c r="C77" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D77" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>69</v>
-      </c>
-      <c r="B78" s="3" t="s">
+      <c r="A78" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C78" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
+      <c r="C78" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D78" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>69</v>
-      </c>
-      <c r="B79" s="3" t="s">
+      <c r="A79" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C79" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D79">
-        <v>1</v>
+      <c r="C79" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D79" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>75</v>
+      <c r="A80" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>4</v>
@@ -3384,83 +3793,83 @@
       <c r="C80" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>75</v>
+      <c r="A81" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D81">
+        <v>80</v>
+      </c>
+      <c r="D81" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>75</v>
+      <c r="A82" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D82">
+        <v>81</v>
+      </c>
+      <c r="D82" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>75</v>
+      <c r="A83" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D83">
+        <v>82</v>
+      </c>
+      <c r="D83" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>75</v>
+      <c r="A84" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D84">
+        <v>81</v>
+      </c>
+      <c r="D84" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>75</v>
+      <c r="A85" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D85">
+        <v>82</v>
+      </c>
+      <c r="D85" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>80</v>
+      <c r="A86" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>4</v>
@@ -3468,251 +3877,251 @@
       <c r="C86" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>80</v>
+      <c r="A87" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D87">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="D87" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>80</v>
+      <c r="A88" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D88">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="D88" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>80</v>
-      </c>
-      <c r="B89" s="3" t="s">
+      <c r="A89" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D89" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>80</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D90">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="D90" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>80</v>
+      <c r="A91" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D91">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="D91" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>86</v>
+      <c r="A92" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D92">
+        <v>5</v>
+      </c>
+      <c r="D92" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>86</v>
+      <c r="A93" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D93">
+        <v>89</v>
+      </c>
+      <c r="D93" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>86</v>
-      </c>
-      <c r="B94" s="3" t="s">
+      <c r="A94" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D94" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>86</v>
-      </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D95">
-        <v>1</v>
+      <c r="C95" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D95" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>86</v>
-      </c>
-      <c r="B96" s="3" t="s">
+      <c r="A96" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D96">
-        <v>1</v>
+      <c r="C96" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D96" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>86</v>
-      </c>
-      <c r="B97" s="3" t="s">
+      <c r="A97" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D97">
-        <v>1</v>
+      <c r="C97" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D97" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>92</v>
+      <c r="A98" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D98">
+        <v>15</v>
+      </c>
+      <c r="D98" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>92</v>
+      <c r="A99" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D99" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>92</v>
-      </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D100">
+      <c r="C100" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D100" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>92</v>
-      </c>
-      <c r="B101" s="3" t="s">
+      <c r="A101" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D101">
-        <v>1</v>
+      <c r="C101" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D101" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>92</v>
+      <c r="A102" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D102">
-        <v>0</v>
+        <v>98</v>
+      </c>
+      <c r="D102" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>92</v>
-      </c>
-      <c r="B103" s="3" t="s">
+      <c r="A103" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C103" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D103">
+      <c r="C103" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D103" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>97</v>
+      <c r="A104" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>4</v>
@@ -3720,83 +4129,83 @@
       <c r="C104" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>97</v>
-      </c>
-      <c r="B105" s="3" t="s">
+      <c r="A105" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C105" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D105">
+      <c r="C105" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D106" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>97</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D106">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D107" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>97</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C107" s="3" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D107">
+      <c r="B108" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D108" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>97</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D108">
-        <v>1</v>
-      </c>
-    </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>97</v>
-      </c>
-      <c r="B109" s="3" t="s">
+      <c r="A109" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D109">
-        <v>1</v>
+      <c r="C109" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D109" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>103</v>
+      <c r="A110" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>4</v>
@@ -3804,83 +4213,83 @@
       <c r="C110" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>103</v>
-      </c>
-      <c r="B111" s="2" t="s">
+      <c r="A111" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D111">
-        <v>2</v>
+      <c r="C111" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D111" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>103</v>
-      </c>
-      <c r="B112" s="2" t="s">
+      <c r="A112" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D112">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>103</v>
-      </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D113">
+      <c r="C113" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D113" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>103</v>
-      </c>
-      <c r="B114" s="3" t="s">
+      <c r="A114" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D114">
-        <v>1</v>
+      <c r="C114" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D114" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>103</v>
-      </c>
-      <c r="B115" s="2" t="s">
+      <c r="A115" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D115">
-        <v>2</v>
+      <c r="C115" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D115" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>107</v>
+      <c r="A116" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>4</v>
@@ -3888,165 +4297,670 @@
       <c r="C116" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>107</v>
+      <c r="A117" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D117">
+        <v>112</v>
+      </c>
+      <c r="D117" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>107</v>
-      </c>
-      <c r="B118" s="3" t="s">
+      <c r="A118" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D118">
+      <c r="C118" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D118" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>107</v>
-      </c>
-      <c r="B119" s="2" t="s">
+      <c r="A119" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D119">
-        <v>2</v>
+      <c r="C119" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D119" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>107</v>
-      </c>
-      <c r="B120" s="2" t="s">
+      <c r="A120" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D120">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>107</v>
-      </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C121" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D121">
+      <c r="C121" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D121" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>113</v>
+      <c r="A122" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C122" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D122" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D123" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D124" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D125" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D127" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>113</v>
-      </c>
-      <c r="B123" s="3" t="s">
+      <c r="D128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B129" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C123" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D123">
+      <c r="C129" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D130" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D131" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>113</v>
-      </c>
-      <c r="B124" s="3" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D132" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D133" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D124">
+      <c r="C136" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D136" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D137" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D138" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D139" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D141" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D142" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D143" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>113</v>
-      </c>
-      <c r="B125" s="3" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D144" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D145" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D146" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D147" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D148" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C125" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D125">
+      <c r="C149" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D149" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D150" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D151" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>113</v>
-      </c>
-      <c r="B126" s="2" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D152" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D153" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D154" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D155" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C126" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D126">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>113</v>
-      </c>
-      <c r="B127" s="3" t="s">
+      <c r="C156" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D156" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C127" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D127">
+      <c r="C157" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D157" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D158" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D159" s="1">
         <v>1</v>
       </c>
     </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D160" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D161" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D162" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D163" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D163" xr:uid="{BBAC580C-6DBF-4BD9-8363-2556C5C8014C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Push Inference results section in readme
</commit_message>
<xml_diff>
--- a/data/inference_images/inference_results.xlsx
+++ b/data/inference_images/inference_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Vie Professionnelle\GitHub Projects\CV-image-captioning-clip-gpt2-aws\data\inference_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4D144D-5C0E-47EC-9A67-7383BBE5BC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4060C1-DBDC-458F-898A-1EB4C2C51B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B9F52076-50CF-4234-A6EE-BD5871CA9C28}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{B9F52076-50CF-4234-A6EE-BD5871CA9C28}"/>
   </bookViews>
   <sheets>
     <sheet name="inference_results" sheetId="1" r:id="rId1"/>
@@ -2614,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBAC580C-6DBF-4BD9-8363-2556C5C8014C}">
   <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>